<commit_message>
Correction of dep vals
</commit_message>
<xml_diff>
--- a/Nil/Summary.xlsx
+++ b/Nil/Summary.xlsx
@@ -480,7 +480,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,8 +600,8 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="4"/>
       <c r="G7" s="2">
-        <f>SUM(G3:G4)</f>
-        <v>118353</v>
+        <f>SUM(B3:B4)</f>
+        <v>115000</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="6"/>
@@ -639,7 +639,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="7">
-        <v>1077424</v>
+        <v>975000</v>
       </c>
       <c r="C15" s="4"/>
       <c r="H15" s="7"/>
@@ -649,7 +649,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="7">
-        <v>442538</v>
+        <v>430000</v>
       </c>
       <c r="C16" s="4"/>
       <c r="H16" s="7"/>
@@ -659,7 +659,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="7">
-        <v>118353</v>
+        <v>115000</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
       </c>
       <c r="B20" s="2">
         <f>SUM(B15:B17)</f>
-        <v>1638315</v>
+        <v>1520000</v>
       </c>
       <c r="F20" s="7"/>
     </row>
@@ -690,7 +690,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,8 +840,8 @@
       <c r="C8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="2">
-        <f>SUM(G3:G5)</f>
-        <v>442538</v>
+        <f>SUM(B3:B5)</f>
+        <v>430000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="7"/>
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1098,7 @@
         <v>42736</v>
       </c>
       <c r="G3" s="7">
-        <v>500000</v>
+        <v>400000</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>13</v>
@@ -1249,8 +1249,8 @@
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="2">
-        <f>SUM(G3:G6)</f>
-        <v>1077424</v>
+        <f>SUM(B3:B6)</f>
+        <v>975000</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="7"/>

</xml_diff>

<commit_message>
Updated for trd a/c
</commit_message>
<xml_diff>
--- a/Nil/Summary.xlsx
+++ b/Nil/Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t>bk</t>
   </si>
@@ -498,7 +498,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,15 +1347,23 @@
       <c r="E7" s="3">
         <v>390</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="4">
+        <v>42750</v>
+      </c>
+      <c r="G7" s="7">
+        <v>225000</v>
+      </c>
       <c r="H7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7">
+        <v>1472</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>

<commit_message>
Updated IC as on 03-Aug
</commit_message>
<xml_diff>
--- a/Nil/Summary.xlsx
+++ b/Nil/Summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="270" windowWidth="14895" windowHeight="7875"/>
+    <workbookView xWindow="360" yWindow="270" windowWidth="14895" windowHeight="7875" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CT-IP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
   <si>
     <t>bk</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>0X0XX8502600</t>
+  </si>
+  <si>
+    <t>344110000113</t>
+  </si>
+  <si>
+    <t>344110000130</t>
+  </si>
+  <si>
+    <t>344110000134</t>
+  </si>
+  <si>
+    <t>jun</t>
+  </si>
+  <si>
+    <t>jul</t>
   </si>
 </sst>
 </file>
@@ -144,13 +159,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,24 +237,27 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -600,41 +618,41 @@
       <c r="F2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="15">
         <v>100000</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="16">
         <v>42467</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="14">
         <v>7</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="14">
         <v>151</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="16">
         <v>42618</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="15">
         <v>102916</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="19"/>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="4"/>
@@ -922,7 +940,7 @@
       <c r="F7" s="4">
         <v>42573</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="19">
         <v>154374</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -952,7 +970,7 @@
       <c r="F8" s="4">
         <v>42573</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="19">
         <v>308748</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -982,7 +1000,7 @@
       <c r="F9" s="4">
         <v>42618</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="19">
         <v>82333</v>
       </c>
       <c r="H9" s="3" t="s">
@@ -1012,7 +1030,7 @@
       <c r="F10" s="4">
         <v>42618</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="19">
         <v>30875</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1042,7 +1060,7 @@
       <c r="F11" s="4">
         <v>42629</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="19">
         <v>823328</v>
       </c>
       <c r="H11" s="3" t="s">
@@ -1248,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,12 +1279,12 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="15" style="13" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="23" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1288,17 +1306,23 @@
       <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="21" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="7"/>
       <c r="C2" s="11"/>
@@ -1306,52 +1330,56 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="3"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="15">
-        <v>50000</v>
-      </c>
-      <c r="C3" s="16">
-        <v>42175</v>
-      </c>
-      <c r="D3" s="14">
-        <v>8.5</v>
-      </c>
-      <c r="E3" s="14">
+      <c r="B3" s="7">
+        <v>500000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>42346</v>
+      </c>
+      <c r="D3" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="E3" s="3">
         <v>390</v>
       </c>
-      <c r="F3" s="16">
-        <v>42565</v>
-      </c>
-      <c r="G3" s="15">
-        <v>50000</v>
-      </c>
-      <c r="H3" s="14">
-        <v>4710076570</v>
-      </c>
-      <c r="I3" s="15">
-        <v>352</v>
-      </c>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14" t="s">
+      <c r="F3" s="4">
+        <v>42736</v>
+      </c>
+      <c r="G3" s="7">
+        <v>500000</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="7">
+        <v>3270</v>
+      </c>
+      <c r="J3" s="13">
+        <v>1992</v>
+      </c>
+      <c r="K3" s="13">
+        <v>2943</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7">
-        <v>500000</v>
+        <v>400000</v>
       </c>
       <c r="C4" s="4">
         <v>42346</v>
@@ -1366,29 +1394,31 @@
         <v>42736</v>
       </c>
       <c r="G4" s="7">
-        <v>500000</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>13</v>
+        <v>400000</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="I4" s="7">
-        <v>3270</v>
-      </c>
-      <c r="J4" s="3"/>
+        <v>7900</v>
+      </c>
+      <c r="J4" s="13">
+        <v>7110</v>
+      </c>
       <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="7">
-        <v>400000</v>
+        <v>225000</v>
       </c>
       <c r="C5" s="4">
-        <v>42346</v>
+        <v>42360</v>
       </c>
       <c r="D5" s="3">
         <v>7.9</v>
@@ -1397,92 +1427,102 @@
         <v>390</v>
       </c>
       <c r="F5" s="4">
-        <v>42736</v>
+        <v>42750</v>
       </c>
       <c r="G5" s="7">
-        <v>400000</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>22</v>
+        <v>225000</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>21</v>
       </c>
       <c r="I5" s="7">
-        <v>7900</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1472</v>
+      </c>
+      <c r="J5" s="13">
+        <v>1325</v>
+      </c>
+      <c r="K5" s="13">
+        <v>1325</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="7">
-        <v>225000</v>
+        <v>125000</v>
       </c>
       <c r="C6" s="4">
-        <v>42360</v>
+        <v>42480</v>
       </c>
       <c r="D6" s="3">
-        <v>7.9</v>
+        <v>7.5</v>
       </c>
       <c r="E6" s="3">
         <v>390</v>
       </c>
       <c r="F6" s="4">
-        <v>42750</v>
+        <v>42870</v>
       </c>
       <c r="G6" s="7">
-        <v>225000</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="7">
-        <v>1472</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
+        <v>125000</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="20">
+        <v>776</v>
+      </c>
+      <c r="J6">
+        <v>699</v>
+      </c>
+      <c r="K6">
+        <v>698</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="7">
-        <v>120000</v>
+        <v>150000</v>
       </c>
       <c r="C7" s="4">
-        <v>42376</v>
+        <v>42542</v>
       </c>
       <c r="D7" s="3">
-        <v>7.75</v>
+        <v>7.5</v>
       </c>
       <c r="E7" s="3">
-        <v>5</v>
+        <v>390</v>
       </c>
       <c r="F7" s="4">
-        <v>44203</v>
+        <v>42932</v>
       </c>
       <c r="G7" s="7">
-        <v>120000</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="7">
-        <v>770</v>
+        <v>125000</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="20">
+        <v>932</v>
       </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>839</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -1490,7 +1530,7 @@
         <v>125000</v>
       </c>
       <c r="C8" s="4">
-        <v>42480</v>
+        <v>42562</v>
       </c>
       <c r="D8" s="3">
         <v>7.5</v>
@@ -1499,82 +1539,109 @@
         <v>390</v>
       </c>
       <c r="F8" s="4">
-        <v>42870</v>
+        <v>42932</v>
       </c>
       <c r="G8" s="7">
         <v>125000</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="15">
+      <c r="H8" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="20">
         <v>776</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="K8" s="24">
+        <v>700</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="11"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
       <c r="B10" s="7"/>
-      <c r="C10" s="11"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="2">
-        <f>SUM(B3:B8)</f>
-        <v>1420000</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="7"/>
+        <f>SUM(G3:G8)</f>
+        <v>1500000</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="11"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="7"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="20"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7">
+        <v>120000</v>
+      </c>
+      <c r="C12" s="4">
+        <v>42376</v>
+      </c>
+      <c r="D12" s="3">
+        <v>7.75</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>44203</v>
+      </c>
+      <c r="G12" s="7">
+        <v>120000</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="7">
+        <v>770</v>
+      </c>
+      <c r="J12">
+        <v>770</v>
+      </c>
+      <c r="K12">
+        <v>693</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="11"/>
@@ -1582,106 +1649,170 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="7"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="11"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="2">
+        <f>SUM(G10:G12)</f>
+        <v>1620000</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20">
+        <f>SUM(I3,I5,I6,I7,I8,I12)</f>
+        <v>7996</v>
+      </c>
       <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="K14" s="2">
+        <f>SUM(K3:K12)</f>
+        <v>7198</v>
+      </c>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
       <c r="B15" s="7"/>
       <c r="C15" s="11"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="7"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="11"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="21"/>
       <c r="I16" s="7"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="3"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="11"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="7"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="11"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="7"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="11"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="21"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I23" s="1"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="7"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="M23" s="3"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>